<commit_message>
Second round of testing done
</commit_message>
<xml_diff>
--- a/Match3_Toolkit/tests/test_results.xlsx
+++ b/Match3_Toolkit/tests/test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\GameLab\BA_Match3_Toolkit\Match3_Toolkit\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147AE107-57E7-4D8C-AA30-09FE0A167E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025402D2-C4C9-45FA-80B9-ED1927005B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t xml:space="preserve">					</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Difficulty</t>
+  </si>
+  <si>
+    <t>blocked</t>
+  </si>
+  <si>
+    <t>blocked + paint</t>
+  </si>
+  <si>
+    <t>difficulty doesnt rise much to 3</t>
   </si>
 </sst>
 </file>
@@ -1304,9 +1313,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Difficulties!$A$12:$A$23</c:f>
+              <c:f>Difficulties!$A$12:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>score</c:v>
                 </c:pt>
@@ -1342,16 +1351,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>time + removable</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>blocked</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>blocked + paint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Difficulties!$B$12:$B$23</c:f>
+              <c:f>Difficulties!$B$12:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>150.61017659999999</c:v>
                 </c:pt>
@@ -1387,6 +1402,12 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>41.9432586</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>188.7527102</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58.246919499999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1423,9 +1444,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Difficulties!$A$12:$A$23</c:f>
+              <c:f>Difficulties!$A$12:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>score</c:v>
                 </c:pt>
@@ -1461,16 +1482,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>time + removable</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>blocked</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>blocked + paint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Difficulties!$C$12:$C$23</c:f>
+              <c:f>Difficulties!$C$12:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>150.61017659999999</c:v>
                 </c:pt>
@@ -1506,6 +1533,12 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>173.8477948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>200.4053404</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>111.0645395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,9 +1575,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Difficulties!$A$12:$A$23</c:f>
+              <c:f>Difficulties!$A$12:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>score</c:v>
                 </c:pt>
@@ -1580,16 +1613,22 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>time + removable</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>blocked</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>blocked + paint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Difficulties!$D$12:$D$23</c:f>
+              <c:f>Difficulties!$D$12:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>150.61017659999999</c:v>
                 </c:pt>
@@ -1625,6 +1664,12 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>210.5218366</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>236.76121449999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>122.9209477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3291,10 +3336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC0C93A-C015-4CA3-AD87-45AB0AC8DE29}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3386,7 +3431,7 @@
         <v>7</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H65" si="0" xml:space="preserve"> 100 + (B5 + C5 + D5) - 100 * F5</f>
+        <f t="shared" ref="H5:H68" si="0" xml:space="preserve"> 100 + (B5 + C5 + D5) - 100 * F5</f>
         <v>156.53526109999996</v>
       </c>
     </row>
@@ -4366,7 +4411,7 @@
         <v>173.8477948</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>112.44995</v>
       </c>
@@ -4385,6 +4430,138 @@
       <c r="H65">
         <f t="shared" si="0"/>
         <v>210.5218366</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68">
+        <v>103.0564028</v>
+      </c>
+      <c r="C68">
+        <v>4.9963074000000001</v>
+      </c>
+      <c r="D68">
+        <v>20.7</v>
+      </c>
+      <c r="E68">
+        <v>144.9</v>
+      </c>
+      <c r="F68">
+        <v>0.4</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="0"/>
+        <v>188.7527102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>112.772909</v>
+      </c>
+      <c r="C69">
+        <v>4.9324313999999996</v>
+      </c>
+      <c r="D69">
+        <v>22.7</v>
+      </c>
+      <c r="E69">
+        <v>169.5</v>
+      </c>
+      <c r="F69">
+        <v>0.4</v>
+      </c>
+      <c r="H69">
+        <f t="shared" ref="H69:H74" si="1" xml:space="preserve"> 100 + (B69 + C69 + D69) - 100 * F69</f>
+        <v>200.4053404</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>117.1713815</v>
+      </c>
+      <c r="C70">
+        <v>4.7898329999999998</v>
+      </c>
+      <c r="D70">
+        <v>24.8</v>
+      </c>
+      <c r="E70">
+        <v>147.4</v>
+      </c>
+      <c r="F70">
+        <v>0.1</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="1"/>
+        <v>236.76121449999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72">
+        <v>45.0143445</v>
+      </c>
+      <c r="C72">
+        <v>5.5325749999999996</v>
+      </c>
+      <c r="D72">
+        <v>7.7</v>
+      </c>
+      <c r="E72">
+        <v>86.5</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="1"/>
+        <v>58.24691949999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>73.306995499999999</v>
+      </c>
+      <c r="C73">
+        <v>5.2575440000000002</v>
+      </c>
+      <c r="D73">
+        <v>12.5</v>
+      </c>
+      <c r="E73">
+        <v>103.6</v>
+      </c>
+      <c r="F73">
+        <v>0.8</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="1"/>
+        <v>111.0645395</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>91.415329799999995</v>
+      </c>
+      <c r="C74">
+        <v>5.7056179</v>
+      </c>
+      <c r="D74">
+        <v>15.8</v>
+      </c>
+      <c r="E74">
+        <v>125.6</v>
+      </c>
+      <c r="F74">
+        <v>0.9</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>122.9209477</v>
       </c>
     </row>
   </sheetData>
@@ -4395,10 +4572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4740,12 +4917,66 @@
         <v>19</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>188.7527102</v>
+      </c>
+      <c r="C24">
+        <v>200.4053404</v>
+      </c>
+      <c r="D24">
+        <v>236.76121449999999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>58.246919499999997</v>
+      </c>
+      <c r="C25">
+        <v>111.0645395</v>
+      </c>
+      <c r="D25">
+        <v>122.9209477</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{5B2E51A5-F173-4F5B-964B-EE624100270E}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Difficulties!B24:D24</xm:f>
+              <xm:sqref>E24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Difficulties!B25:D25</xm:f>
+              <xm:sqref>E25</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{2314AD01-79D9-42D3-BBB0-6F44CFBD3252}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>

</xml_diff>

<commit_message>
some more testing and smaller fixes
</commit_message>
<xml_diff>
--- a/Match3_Toolkit/tests/test_results.xlsx
+++ b/Match3_Toolkit/tests/test_results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\GameLab\BA_Match3_Toolkit\Match3_Toolkit\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\_GAMELAB\BachelorThesis\BA_Match3_Toolkit\Match3_Toolkit\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025402D2-C4C9-45FA-80B9-ED1927005B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39013CAD-EDBC-41BB-BF78-D56CF514B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test results" sheetId="2" r:id="rId1"/>
+    <sheet name="results" sheetId="2" r:id="rId1"/>
     <sheet name="Difficulties" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t xml:space="preserve">					</t>
   </si>
@@ -145,6 +145,24 @@
   </si>
   <si>
     <t>difficulty doesnt rise much to 3</t>
+  </si>
+  <si>
+    <t>full clear</t>
+  </si>
+  <si>
+    <t>original diff</t>
+  </si>
+  <si>
+    <t>normalization of new diff</t>
+  </si>
+  <si>
+    <t>normalization of old diff</t>
+  </si>
+  <si>
+    <t>Normalization of move time</t>
+  </si>
+  <si>
+    <t>shielded + paint</t>
   </si>
 </sst>
 </file>
@@ -838,19 +856,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>105.7337775</c:v>
+                  <c:v>0.57612907999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.53526110000001</c:v>
+                  <c:v>0.32790338594496743</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.579206800000001</c:v>
+                  <c:v>0.30964405198864697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.614393399999997</c:v>
+                  <c:v>0.85855333849195425</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.479630100000001</c:v>
+                  <c:v>0.31047853725415908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,19 +933,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>105.7337775</c:v>
+                  <c:v>0.57612907999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.53526110000001</c:v>
+                  <c:v>0.32790338594496743</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.346110999999993</c:v>
+                  <c:v>0.69434957845988809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>154.5535778</c:v>
+                  <c:v>1.3746685270991623</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.045926100000003</c:v>
+                  <c:v>0.64535056745855879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -992,19 +1010,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>105.7337775</c:v>
+                  <c:v>0.57612907999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.53526110000001</c:v>
+                  <c:v>0.32790338594496743</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81.726435699999996</c:v>
+                  <c:v>0.7424989293480273</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>174.97139390000001</c:v>
+                  <c:v>1.5347830370561719</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>131.1202792</c:v>
+                  <c:v>1.1229533094079622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,7 +1264,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Swapping scenarios</a:t>
+              <a:t>Swapping</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> scenarios</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1313,9 +1335,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Difficulties!$A$12:$A$25</c:f>
+              <c:f>Difficulties!$A$12:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>score</c:v>
                 </c:pt>
@@ -1357,64 +1379,70 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>blocked + paint</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>shielded + paint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Difficulties!$B$12:$B$25</c:f>
+              <c:f>Difficulties!$B$12:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>150.61017659999999</c:v>
+                  <c:v>0.74171399187828646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151.46573029999999</c:v>
+                  <c:v>0.82362130318453575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153.71579349999999</c:v>
+                  <c:v>0.60010891510653153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.92256209999999</c:v>
+                  <c:v>1.4042359345094091</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>152.960701</c:v>
+                  <c:v>1.9646247544483977</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.539748699999997</c:v>
+                  <c:v>0.91444113536024751</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.124824099999998</c:v>
+                  <c:v>0.87482783034631073</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.830330700000005</c:v>
+                  <c:v>1.342800333716601</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>127.2022891</c:v>
+                  <c:v>1.6989176241456923</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>203.9867897</c:v>
+                  <c:v>2.3253540748570423</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>122.237178</c:v>
+                  <c:v>1.4716667097826732</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41.9432586</c:v>
+                  <c:v>0.81409087816313097</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>188.7527102</c:v>
+                  <c:v>2.0634367178920114</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>58.246919499999997</c:v>
+                  <c:v>1.0879060583376314</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1117900022085325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-35E3-48A9-B432-D9D4938577BE}"/>
+              <c16:uniqueId val="{00000000-E421-4B4F-82F2-4E22C31EBA23}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1444,9 +1472,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Difficulties!$A$12:$A$25</c:f>
+              <c:f>Difficulties!$A$12:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>score</c:v>
                 </c:pt>
@@ -1488,64 +1516,70 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>blocked + paint</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>shielded + paint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Difficulties!$C$12:$C$25</c:f>
+              <c:f>Difficulties!$C$12:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>150.61017659999999</c:v>
+                  <c:v>0.74171399187828646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151.3650447</c:v>
+                  <c:v>0.92011433031608902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151.3374039</c:v>
+                  <c:v>0.91048037733076315</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>248.2098958</c:v>
+                  <c:v>2.6454703918131806</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>219.53444160000001</c:v>
+                  <c:v>2.5080180089992954</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.625420899999995</c:v>
+                  <c:v>1.1896652524711104</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>133.4749631</c:v>
+                  <c:v>1.685674910116761</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>164.90622809999999</c:v>
+                  <c:v>2.0277442104058219</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>217.07579999999999</c:v>
+                  <c:v>2.4933072691980787</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>247.92093080000001</c:v>
+                  <c:v>2.6478846944655028</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>233.1318095</c:v>
+                  <c:v>2.7199752044534931</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>173.8477948</c:v>
+                  <c:v>2.1014745495051614</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200.4053404</c:v>
+                  <c:v>2.1315252448614412</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>111.0645395</c:v>
+                  <c:v>1.4682105594929065</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2018569416666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-35E3-48A9-B432-D9D4938577BE}"/>
+              <c16:uniqueId val="{00000001-E421-4B4F-82F2-4E22C31EBA23}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1575,9 +1609,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Difficulties!$A$12:$A$25</c:f>
+              <c:f>Difficulties!$A$12:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>score</c:v>
                 </c:pt>
@@ -1619,64 +1653,70 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>blocked + paint</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>shielded + paint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Difficulties!$D$12:$D$25</c:f>
+              <c:f>Difficulties!$D$12:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>150.61017659999999</c:v>
+                  <c:v>0.74171399187828646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150.0611615</c:v>
+                  <c:v>0.93566517060549681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>147.81369000000001</c:v>
+                  <c:v>1.1191655581289153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>248.3982963</c:v>
+                  <c:v>2.6227971109281221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>234.25456199999999</c:v>
+                  <c:v>2.6567175277392403</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>148.18629569999999</c:v>
+                  <c:v>1.7524062179739368</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>207.17385379999999</c:v>
+                  <c:v>2.2961140965178499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>244.07273889999999</c:v>
+                  <c:v>2.9608404631404954</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>243.47557330000001</c:v>
+                  <c:v>2.7197363307464149</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>235.3129453</c:v>
+                  <c:v>2.7236794981334151</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>206.68982539999999</c:v>
+                  <c:v>2.362302410485241</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>210.5218366</c:v>
+                  <c:v>2.5586365037144478</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>236.76121449999999</c:v>
+                  <c:v>2.43942028006032</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>122.9209477</c:v>
+                  <c:v>1.6094798116665516</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.092725887194808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-35E3-48A9-B432-D9D4938577BE}"/>
+              <c16:uniqueId val="{00000002-E421-4B4F-82F2-4E22C31EBA23}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1690,11 +1730,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2098451872"/>
-        <c:axId val="118642624"/>
+        <c:axId val="457521472"/>
+        <c:axId val="457527952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098451872"/>
+        <c:axId val="457521472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1777,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118642624"/>
+        <c:crossAx val="457527952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1745,7 +1785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118642624"/>
+        <c:axId val="457527952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1796,7 +1836,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098451872"/>
+        <c:crossAx val="457521472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3003,22 +3043,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>533401</xdr:colOff>
+      <xdr:colOff>552449</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3">
+        <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F94450F-BDD6-9AE5-4D4E-05C63BB0E10A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{579F8A1D-E40F-D47F-C210-A6757E8B1572}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3336,10 +3376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC0C93A-C015-4CA3-AD87-45AB0AC8DE29}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,14 +3391,18 @@
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>27</v>
       </c>
@@ -3380,8 +3424,20 @@
       <c r="H2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3401,19 +3457,35 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="H3">
+        <f>B3/120 + N3 + (1 - F3)</f>
+        <v>0.57612907999999996</v>
+      </c>
+      <c r="J3">
         <f xml:space="preserve"> 100 + (B3 + C3 + D3) - 100 * F3</f>
         <v>105.7337775</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f>(H3 - $H$15)/($H$49 - $H$15)</f>
+        <v>0.10023179858992345</v>
+      </c>
+      <c r="L3">
+        <f>(J3 - $J$7)/($J$33 - $J$7)</f>
+        <v>0.37925088679100133</v>
+      </c>
+      <c r="N3">
+        <f>(C3 - $C$3)/($C$77 - $C$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>120.01109409999999</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>3.6241669999999999</v>
@@ -3431,11 +3503,27 @@
         <v>7</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H68" si="0" xml:space="preserve"> 100 + (B5 + C5 + D5) - 100 * F5</f>
-        <v>156.53526109999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <f xml:space="preserve"> N5 + (1 - E5/$E$5)</f>
+        <v>0.32790338594496743</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J65" si="0" xml:space="preserve"> 100 + (B5 + C5 + D5) - 100 * F5</f>
+        <v>156.52416700000003</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K65" si="1">(H5 - $H$15)/($H$49 - $H$15)</f>
+        <v>6.57451668038927E-3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L65" si="2">(J5 - $J$7)/($J$33 - $J$7)</f>
+        <v>0.60026396853331521</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N4:N67" si="3">(C5 - $C$3)/($C$77 - $C$3)</f>
+        <v>0.32790338594496743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3455,11 +3543,27 @@
         <v>1</v>
       </c>
       <c r="H7">
+        <f t="shared" ref="H7:H65" si="4">B7/120 + N7 + (1 - F7)</f>
+        <v>0.30964405198864697</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>18.579206800000009</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>-3.1485709833121712E-4</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>0.21015327698864694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>50.282636199999999</v>
       </c>
@@ -3476,11 +3580,27 @@
         <v>1</v>
       </c>
       <c r="H8">
+        <f t="shared" si="4"/>
+        <v>0.69434957845988809</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>68.346111000000008</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.14483721542194827</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>0.2165594116189343</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>0.27532761012655477</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>60.026848299999997</v>
       </c>
@@ -3497,11 +3617,27 @@
         <v>1</v>
       </c>
       <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0.7424989293480273</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>81.726435699999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.1630043006105257</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>0.27478355255921588</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>0.24227519351469393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3521,11 +3657,27 @@
         <v>0.9</v>
       </c>
       <c r="H11">
+        <f t="shared" si="4"/>
+        <v>0.85855333849195425</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>90.614393399999983</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.20679243686860146</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0.31345927332076512</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>0.26694949932528766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>85.140496400000004</v>
       </c>
@@ -3542,11 +3694,27 @@
         <v>0.6</v>
       </c>
       <c r="H12">
+        <f t="shared" si="4"/>
+        <v>1.3746685270991623</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>154.5535778</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>0.4015262894667172</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0.59168899999640079</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>0.26516439043249562</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>101.5421154</v>
       </c>
@@ -3557,17 +3725,33 @@
         <v>30</v>
       </c>
       <c r="E13" s="3">
-        <v>30164.9</v>
+        <v>164.9</v>
       </c>
       <c r="F13">
         <v>0.6</v>
       </c>
       <c r="H13">
+        <f t="shared" si="4"/>
+        <v>1.5347830370561719</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>174.97139390000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0.46193860840065448</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>0.68053660489041001</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>0.2885987420561717</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3587,11 +3771,27 @@
         <v>1</v>
       </c>
       <c r="H15">
+        <f t="shared" si="4"/>
+        <v>0.31047853725415908</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>32.479630100000008</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>6.0487336704824105E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>0.12844121975415909</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>53.456555000000002</v>
       </c>
@@ -3608,11 +3808,27 @@
         <v>1</v>
       </c>
       <c r="H16">
+        <f t="shared" si="4"/>
+        <v>0.64535056745855879</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>74.045926100000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>0.12634954755940042</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>0.24136201134328517</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>0.19987927579189213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>90.175843</v>
       </c>
@@ -3629,16 +3845,32 @@
         <v>0.9</v>
       </c>
       <c r="H17">
+        <f t="shared" si="4"/>
+        <v>1.1229533094079622</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>131.1202792</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>0.30655238600369444</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>0.4897196000772715</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>0.27148795107462903</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>27</v>
       </c>
@@ -3657,16 +3889,13 @@
       <c r="G20" t="s">
         <v>32</v>
       </c>
-      <c r="H20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21">
-        <v>120.01204610000001</v>
+        <v>120</v>
       </c>
       <c r="C21">
         <v>4.2981305000000001</v>
@@ -3684,16 +3913,32 @@
         <v>7</v>
       </c>
       <c r="H21">
+        <f>N21 + (1 - E21/$E$5)</f>
+        <v>0.74171399187828646</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="0"/>
-        <v>150.61017660000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>150.5981305</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>0.16270813824037003</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>0.57447697216892546</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>0.46382672345101017</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="B23">
-        <v>120.0093598</v>
+        <v>120</v>
       </c>
       <c r="C23">
         <v>4.3563704999999997</v>
@@ -3711,13 +3956,29 @@
         <v>7</v>
       </c>
       <c r="H23">
+        <f t="shared" ref="H23:H29" si="5">N23 + (1 - E23/$E$5)</f>
+        <v>0.82362130318453575</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="0"/>
-        <v>151.46573029999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>151.45637049999999</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>0.19361233683538184</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>0.57821158159290953</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="3"/>
+        <v>0.47557242655859966</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>120.0113377</v>
+        <v>120</v>
       </c>
       <c r="C24">
         <v>4.4537069999999996</v>
@@ -3735,13 +3996,29 @@
         <v>7</v>
       </c>
       <c r="H24">
+        <f t="shared" si="5"/>
+        <v>0.92011433031608902</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="0"/>
-        <v>151.3650447</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>151.35370699999999</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>0.23001982752150163</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>0.57776484399666694</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="3"/>
+        <v>0.49520301774218295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>120.0121098</v>
+        <v>120</v>
       </c>
       <c r="C25">
         <v>4.3490517000000004</v>
@@ -3759,16 +4036,32 @@
         <v>7</v>
       </c>
       <c r="H25">
+        <f t="shared" si="5"/>
+        <v>0.93566517060549681</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="0"/>
-        <v>150.0611615</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>150.04905170000001</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>0.23588726778976132</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>0.57208766980479664</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>0.47409638857948194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
       <c r="B27">
-        <v>120.0132758</v>
+        <v>120</v>
       </c>
       <c r="C27">
         <v>4.0025177000000003</v>
@@ -3786,13 +4079,29 @@
         <v>7</v>
       </c>
       <c r="H27">
+        <f t="shared" si="5"/>
+        <v>0.60010891510653153</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="0"/>
-        <v>153.71579349999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>153.70251769999999</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>0.10927955726481167</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>0.58798563372375345</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>0.40420824502375663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>120.01192159999999</v>
+        <v>120</v>
       </c>
       <c r="C28">
         <v>4.4254822999999996</v>
@@ -3810,13 +4119,29 @@
         <v>7</v>
       </c>
       <c r="H28">
+        <f t="shared" si="5"/>
+        <v>0.91048037733076315</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="0"/>
-        <v>151.3374039</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>151.3254823</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>0.22638487001202712</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>0.57764202493602068</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="3"/>
+        <v>0.48951072813880414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>120.0121068</v>
+        <v>120</v>
       </c>
       <c r="C29">
         <v>4.8015831999999996</v>
@@ -3834,11 +4159,27 @@
         <v>7</v>
       </c>
       <c r="H29">
+        <f t="shared" si="5"/>
+        <v>1.1191655581289153</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="0"/>
-        <v>147.81369000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>147.80158319999998</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>0.3051232410850131</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>0.56230786807077415</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="3"/>
+        <v>0.56536185296533614</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3858,13 +4199,29 @@
         <v>0.8</v>
       </c>
       <c r="H31">
+        <f t="shared" si="4"/>
+        <v>1.4042359345094091</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="0"/>
         <v>105.92256209999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>0.41268227805886354</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>0.38007237815269856</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="3"/>
+        <v>0.63528361617607587</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>120.0111017</v>
+        <v>120</v>
       </c>
       <c r="C32">
         <v>5.1987940999999998</v>
@@ -3879,13 +4236,29 @@
         <v>0</v>
       </c>
       <c r="H32">
+        <f t="shared" si="4"/>
+        <v>2.6454703918131806</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="0"/>
-        <v>248.2098958</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>248.19879409999999</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0.88100867725005194</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>0.99918376521942698</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="3"/>
+        <v>0.64547039181318033</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>120.0119256</v>
+        <v>120</v>
       </c>
       <c r="C33">
         <v>5.0863706999999998</v>
@@ -3900,11 +4273,27 @@
         <v>0</v>
       </c>
       <c r="H33">
+        <f t="shared" si="4"/>
+        <v>2.6227971109281221</v>
+      </c>
+      <c r="J33">
         <f t="shared" si="0"/>
-        <v>248.3982963</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>248.38637070000001</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0.87245389057597311</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="3"/>
+        <v>0.62279711092812229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -3924,11 +4313,27 @@
         <v>0.6</v>
       </c>
       <c r="H35">
+        <f t="shared" si="4"/>
+        <v>1.9646247544483977</v>
+      </c>
+      <c r="J35">
         <f t="shared" si="0"/>
         <v>152.960701</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>0.62412087988362475</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>0.58475763731402108</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="3"/>
+        <v>0.78052256278173104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>110.2171225</v>
       </c>
@@ -3945,11 +4350,27 @@
         <v>0.1</v>
       </c>
       <c r="H36">
+        <f t="shared" si="4"/>
+        <v>2.5080180089992954</v>
+      </c>
+      <c r="J36">
         <f t="shared" si="0"/>
         <v>219.53444160000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>0.82914693660573668</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>0.87445156795653745</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="3"/>
+        <v>0.68954198816596213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>120</v>
       </c>
@@ -3966,11 +4387,27 @@
         <v>0</v>
       </c>
       <c r="H37">
+        <f t="shared" si="4"/>
+        <v>2.6567175277392403</v>
+      </c>
+      <c r="J37">
         <f t="shared" si="0"/>
         <v>234.25456199999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>0.88525229991011511</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>0.93850579564112524</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="3"/>
+        <v>0.65671752773924053</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -3990,11 +4427,27 @@
         <v>1</v>
       </c>
       <c r="H39">
+        <f t="shared" si="4"/>
+        <v>0.91444113536024751</v>
+      </c>
+      <c r="J39">
         <f t="shared" si="0"/>
         <v>51.539748700000018</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>0.22787929158170003</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>0.14342695562938457</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="3"/>
+        <v>0.58927797202691423</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>63.658667000000001</v>
       </c>
@@ -4011,11 +4464,27 @@
         <v>1</v>
       </c>
       <c r="H40">
+        <f t="shared" si="4"/>
+        <v>1.1896652524711104</v>
+      </c>
+      <c r="J40">
         <f t="shared" si="0"/>
         <v>80.625420899999995</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>0.33172326640744848</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>0.26999251479818637</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="3"/>
+        <v>0.65917636080444364</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>86.454532400000005</v>
       </c>
@@ -4032,11 +4501,27 @@
         <v>0.6</v>
       </c>
       <c r="H41">
+        <f t="shared" si="4"/>
+        <v>1.7524062179739368</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="0"/>
         <v>148.18629570000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>0.54404934912335301</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>0.56398193468154112</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="3"/>
+        <v>0.63195178130727014</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -4056,11 +4541,27 @@
         <v>1</v>
       </c>
       <c r="H43">
+        <f t="shared" si="4"/>
+        <v>0.87482783034631073</v>
+      </c>
+      <c r="J43">
         <f t="shared" si="0"/>
         <v>45.124824100000012</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>0.21293291590861557</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>0.11551257519348379</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="3"/>
+        <v>0.59068031701297741</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>83.037028500000005</v>
       </c>
@@ -4077,11 +4578,27 @@
         <v>0.7</v>
       </c>
       <c r="H44">
+        <f t="shared" si="4"/>
+        <v>1.685674910116761</v>
+      </c>
+      <c r="J44">
         <f t="shared" si="0"/>
         <v>133.47496310000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>0.51887116224804186</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>0.49996594688404322</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="3"/>
+        <v>0.6936996726167608</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>111.467213</v>
       </c>
@@ -4098,11 +4615,27 @@
         <v>0.3</v>
       </c>
       <c r="H45">
+        <f t="shared" si="4"/>
+        <v>2.2961140965178499</v>
+      </c>
+      <c r="J45">
         <f t="shared" si="0"/>
         <v>207.17385379999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>0.74919411566767535</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>0.82066478607284177</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="3"/>
+        <v>0.6672206548511832</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -4122,11 +4655,27 @@
         <v>0.9</v>
       </c>
       <c r="H47">
+        <f t="shared" si="4"/>
+        <v>1.342800333716601</v>
+      </c>
+      <c r="J47">
         <f t="shared" si="0"/>
         <v>86.83033069999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>0.38950219831474975</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="2"/>
+        <v>0.29699302119971893</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="3"/>
+        <v>0.73194395621660091</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>92.870161600000003</v>
       </c>
@@ -4143,13 +4692,29 @@
         <v>0.5</v>
       </c>
       <c r="H48">
+        <f t="shared" si="4"/>
+        <v>2.0277442104058219</v>
+      </c>
+      <c r="J48">
         <f t="shared" si="0"/>
         <v>164.90622810000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f t="shared" si="1"/>
+        <v>0.64793628990024565</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="2"/>
+        <v>0.63673829317032882</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="3"/>
+        <v>0.75382619707248832</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>120.010211</v>
+        <v>120</v>
       </c>
       <c r="C49">
         <v>6.7625279000000003</v>
@@ -4164,11 +4729,27 @@
         <v>0</v>
       </c>
       <c r="H49">
+        <f t="shared" si="4"/>
+        <v>2.9608404631404954</v>
+      </c>
+      <c r="J49">
         <f t="shared" si="0"/>
-        <v>244.07273889999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244.06252789999999</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="2"/>
+        <v>0.98118490857020657</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="3"/>
+        <v>0.96084046314049532</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -4188,11 +4769,27 @@
         <v>0.7</v>
       </c>
       <c r="H51">
+        <f t="shared" si="4"/>
+        <v>1.6989176241456923</v>
+      </c>
+      <c r="J51">
         <f t="shared" si="0"/>
         <v>127.2022891</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <f t="shared" si="1"/>
+        <v>0.52386773041467161</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="2"/>
+        <v>0.47267056629821619</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="3"/>
+        <v>0.74552266664569222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>111.801029</v>
       </c>
@@ -4209,13 +4806,29 @@
         <v>0.2</v>
       </c>
       <c r="H52">
+        <f t="shared" si="4"/>
+        <v>2.4933072691980787</v>
+      </c>
+      <c r="J52">
         <f t="shared" si="0"/>
         <v>217.07580000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <f t="shared" si="1"/>
+        <v>0.82359647209840448</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="2"/>
+        <v>0.86375285187530226</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="3"/>
+        <v>0.7616320275314119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>120.0085383</v>
+        <v>120</v>
       </c>
       <c r="C53">
         <v>5.5670349999999997</v>
@@ -4230,11 +4843,27 @@
         <v>0</v>
       </c>
       <c r="H53">
+        <f t="shared" si="4"/>
+        <v>2.7197363307464149</v>
+      </c>
+      <c r="J53">
         <f t="shared" si="0"/>
-        <v>243.47557330000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>243.46703500000001</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="1"/>
+        <v>0.90902973286810618</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="2"/>
+        <v>0.97859363643623987</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="3"/>
+        <v>0.71973633074641474</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -4254,13 +4883,29 @@
         <v>0.3</v>
       </c>
       <c r="H55">
+        <f t="shared" si="4"/>
+        <v>2.3253540748570423</v>
+      </c>
+      <c r="J55">
         <f t="shared" si="0"/>
         <v>203.9867897</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <f t="shared" si="1"/>
+        <v>0.76022656299254932</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="2"/>
+        <v>0.80679635810082762</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="3"/>
+        <v>0.72020898235704245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>120.01016559999999</v>
+        <v>120</v>
       </c>
       <c r="C56">
         <v>5.2107652</v>
@@ -4275,11 +4920,27 @@
         <v>0</v>
       </c>
       <c r="H56">
+        <f t="shared" si="4"/>
+        <v>2.6478846944655028</v>
+      </c>
+      <c r="J56">
         <f t="shared" si="0"/>
-        <v>247.92093079999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>247.91076519999999</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="1"/>
+        <v>0.88191961044326661</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="2"/>
+        <v>0.9979304148228948</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="3"/>
+        <v>0.6478846944655029</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>119.92752280000001</v>
       </c>
@@ -4296,11 +4957,27 @@
         <v>0.1</v>
       </c>
       <c r="H57">
+        <f t="shared" si="4"/>
+        <v>2.7236794981334151</v>
+      </c>
+      <c r="J57">
         <f t="shared" si="0"/>
         <v>235.31294530000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <f t="shared" si="1"/>
+        <v>0.91051751736594666</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="2"/>
+        <v>0.9431113235195363</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="3"/>
+        <v>0.82428347480008202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -4320,11 +4997,27 @@
         <v>0.7</v>
       </c>
       <c r="H59">
+        <f t="shared" si="4"/>
+        <v>1.4716667097826732</v>
+      </c>
+      <c r="J59">
         <f t="shared" si="0"/>
         <v>122.237178</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <f t="shared" si="1"/>
+        <v>0.43812437885825301</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="2"/>
+        <v>0.45106501225134343</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="3"/>
+        <v>0.56206728811600659</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>117.9844672</v>
       </c>
@@ -4341,11 +5034,27 @@
         <v>0.1</v>
       </c>
       <c r="H60">
+        <f t="shared" si="4"/>
+        <v>2.7199752044534931</v>
+      </c>
+      <c r="J60">
         <f t="shared" si="0"/>
         <v>233.1318095</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <f t="shared" si="1"/>
+        <v>0.9091198615802436</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="2"/>
+        <v>0.93362016683414628</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="3"/>
+        <v>0.83677131112015979</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>111.6630895</v>
       </c>
@@ -4362,11 +5071,27 @@
         <v>0.3</v>
       </c>
       <c r="H61">
+        <f t="shared" si="4"/>
+        <v>2.362302410485241</v>
+      </c>
+      <c r="J61">
         <f t="shared" si="0"/>
         <v>206.68982539999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <f t="shared" si="1"/>
+        <v>0.77416742716937015</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="2"/>
+        <v>0.81855854886167012</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="3"/>
+        <v>0.73177666465190749</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -4386,11 +5111,27 @@
         <v>1</v>
       </c>
       <c r="H63">
+        <f t="shared" si="4"/>
+        <v>0.81409087816313097</v>
+      </c>
+      <c r="J63">
         <f t="shared" si="0"/>
         <v>41.943258600000007</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <f t="shared" si="1"/>
+        <v>0.19001644114720423</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="2"/>
+        <v>0.10166807423882923</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="3"/>
+        <v>0.55498132566313096</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>97.951964500000003</v>
       </c>
@@ -4407,11 +5148,27 @@
         <v>0.4</v>
       </c>
       <c r="H64">
+        <f t="shared" si="4"/>
+        <v>2.1014745495051614</v>
+      </c>
+      <c r="J64">
         <f t="shared" si="0"/>
         <v>173.8477948</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <f t="shared" si="1"/>
+        <v>0.67575525997343022</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="2"/>
+        <v>0.67564729212516939</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="3"/>
+        <v>0.68520817867182804</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>112.44995</v>
       </c>
@@ -4428,11 +5185,27 @@
         <v>0.2</v>
       </c>
       <c r="H65">
+        <f t="shared" si="4"/>
+        <v>2.5586365037144478</v>
+      </c>
+      <c r="J65">
         <f t="shared" si="0"/>
         <v>210.5218366</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <f t="shared" si="1"/>
+        <v>0.8482456469444104</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="2"/>
+        <v>0.83523344765493612</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="3"/>
+        <v>0.82155358704778092</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -4452,11 +5225,27 @@
         <v>0.4</v>
       </c>
       <c r="H68">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H68:H78" si="6">B68/120 + N68 + (1 - F68)</f>
+        <v>2.0634367178920114</v>
+      </c>
+      <c r="J68">
+        <f t="shared" ref="J68:J78" si="7" xml:space="preserve"> 100 + (B68 + C68 + D68) - 100 * F68</f>
         <v>188.7527102</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <f t="shared" ref="K68:K78" si="8">(H68 - $H$15)/($H$49 - $H$15)</f>
+        <v>0.66140332137907032</v>
+      </c>
+      <c r="L68">
+        <f t="shared" ref="L68:L78" si="9">(J68 - $J$7)/($J$33 - $J$7)</f>
+        <v>0.74050565052902595</v>
+      </c>
+      <c r="N68">
+        <f t="shared" ref="N68:N78" si="10">(C68 - $C$3)/($C$77 - $C$3)</f>
+        <v>0.60463336122534472</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>112.772909</v>
       </c>
@@ -4473,11 +5262,27 @@
         <v>0.4</v>
       </c>
       <c r="H69">
-        <f t="shared" ref="H69:H74" si="1" xml:space="preserve"> 100 + (B69 + C69 + D69) - 100 * F69</f>
+        <f t="shared" si="6"/>
+        <v>2.1315252448614412</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="7"/>
         <v>200.4053404</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <f t="shared" si="8"/>
+        <v>0.68709359647108803</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="9"/>
+        <v>0.79121177301122414</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="10"/>
+        <v>0.59175100319477469</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>117.1713815</v>
       </c>
@@ -4494,11 +5299,27 @@
         <v>0.1</v>
       </c>
       <c r="H70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
+        <v>2.43942028006032</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="7"/>
         <v>236.76121449999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <f t="shared" si="8"/>
+        <v>0.80326453606678583</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="9"/>
+        <v>0.94941342992658539</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="10"/>
+        <v>0.56299210089365359</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>35</v>
       </c>
@@ -4518,11 +5339,27 @@
         <v>1</v>
       </c>
       <c r="H72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
+        <v>1.0879060583376314</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="7"/>
         <v>58.24691949999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <f t="shared" si="8"/>
+        <v>0.29332881426127655</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="9"/>
+        <v>0.17261303793497615</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="10"/>
+        <v>0.7127865208376315</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>73.306995499999999</v>
       </c>
@@ -4539,11 +5376,27 @@
         <v>0.8</v>
       </c>
       <c r="H73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
+        <v>1.4682105594929065</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="7"/>
         <v>111.0645395</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K73">
+        <f t="shared" si="8"/>
+        <v>0.43682034930062535</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="9"/>
+        <v>0.40244756138344207</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="10"/>
+        <v>0.65731893032623978</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>91.415329799999995</v>
       </c>
@@ -4560,8 +5413,138 @@
         <v>0.9</v>
       </c>
       <c r="H74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
+        <v>1.6094798116665516</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="7"/>
         <v>122.9209477</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="8"/>
+        <v>0.49012222131812405</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="9"/>
+        <v>0.45404041862421674</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="10"/>
+        <v>0.74768539666655176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76">
+        <v>33.733984100000001</v>
+      </c>
+      <c r="C76">
+        <v>5.6212657999999998</v>
+      </c>
+      <c r="D76">
+        <v>5.7</v>
+      </c>
+      <c r="E76">
+        <v>43</v>
+      </c>
+      <c r="F76">
+        <v>0.9</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="6"/>
+        <v>1.1117900022085325</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="7"/>
+        <v>55.055249900000007</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="8"/>
+        <v>0.30234039250560024</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="9"/>
+        <v>0.15872456924742545</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="10"/>
+        <v>0.73067346804186584</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>96.222832999999994</v>
+      </c>
+      <c r="C77">
+        <v>6.9566968999999999</v>
+      </c>
+      <c r="D77">
+        <v>13.6</v>
+      </c>
+      <c r="E77">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="F77">
+        <v>0.6</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="6"/>
+        <v>2.2018569416666667</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="7"/>
+        <v>156.7795299</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="8"/>
+        <v>0.71363023515363511</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="9"/>
+        <v>0.60137517366576743</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>87.756369599999999</v>
+      </c>
+      <c r="C78">
+        <v>6.7654154000000002</v>
+      </c>
+      <c r="D78">
+        <v>12.9</v>
+      </c>
+      <c r="E78">
+        <v>117.7</v>
+      </c>
+      <c r="F78">
+        <v>0.6</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="6"/>
+        <v>2.092725887194808</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="7"/>
+        <v>147.421785</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="8"/>
+        <v>0.67245432879685973</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="9"/>
+        <v>0.56065518591085139</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="10"/>
+        <v>0.96142280719480788</v>
       </c>
     </row>
   </sheetData>
@@ -4572,10 +5555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4607,13 +5590,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>105.7337775</v>
+        <f>results!H3</f>
+        <v>0.57612907999999996</v>
       </c>
       <c r="C3">
-        <v>105.7337775</v>
+        <f>results!H3</f>
+        <v>0.57612907999999996</v>
       </c>
       <c r="D3">
-        <v>105.7337775</v>
+        <f>results!H3</f>
+        <v>0.57612907999999996</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -4624,13 +5610,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>156.53526110000001</v>
+        <f>results!H5</f>
+        <v>0.32790338594496743</v>
       </c>
       <c r="C4">
-        <v>156.53526110000001</v>
+        <f>results!H5</f>
+        <v>0.32790338594496743</v>
       </c>
       <c r="D4">
-        <v>156.53526110000001</v>
+        <f>results!H5</f>
+        <v>0.32790338594496743</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -4641,13 +5630,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>18.579206800000001</v>
+        <f>results!H7</f>
+        <v>0.30964405198864697</v>
       </c>
       <c r="C5">
-        <v>68.346110999999993</v>
+        <f>results!H8</f>
+        <v>0.69434957845988809</v>
       </c>
       <c r="D5">
-        <v>81.726435699999996</v>
+        <f>results!H9</f>
+        <v>0.7424989293480273</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -4658,13 +5650,16 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>90.614393399999997</v>
+        <f>results!H11</f>
+        <v>0.85855333849195425</v>
       </c>
       <c r="C6">
-        <v>154.5535778</v>
+        <f>results!H12</f>
+        <v>1.3746685270991623</v>
       </c>
       <c r="D6">
-        <v>174.97139390000001</v>
+        <f>results!H13</f>
+        <v>1.5347830370561719</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -4675,13 +5670,16 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>32.479630100000001</v>
+        <f>results!H15</f>
+        <v>0.31047853725415908</v>
       </c>
       <c r="C7">
-        <v>74.045926100000003</v>
+        <f>results!H16</f>
+        <v>0.64535056745855879</v>
       </c>
       <c r="D7">
-        <v>131.1202792</v>
+        <f>results!H17</f>
+        <v>1.1229533094079622</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -4718,13 +5716,16 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>150.61017659999999</v>
+        <f>results!H21</f>
+        <v>0.74171399187828646</v>
       </c>
       <c r="C12">
-        <v>150.61017659999999</v>
+        <f>results!H21</f>
+        <v>0.74171399187828646</v>
       </c>
       <c r="D12">
-        <v>150.61017659999999</v>
+        <f>results!H21</f>
+        <v>0.74171399187828646</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -4735,13 +5736,16 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>151.46573029999999</v>
+        <f>results!H23</f>
+        <v>0.82362130318453575</v>
       </c>
       <c r="C13">
-        <v>151.3650447</v>
+        <f>results!H24</f>
+        <v>0.92011433031608902</v>
       </c>
       <c r="D13">
-        <v>150.0611615</v>
+        <f>results!H25</f>
+        <v>0.93566517060549681</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -4752,13 +5756,16 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>153.71579349999999</v>
+        <f>results!H27</f>
+        <v>0.60010891510653153</v>
       </c>
       <c r="C14">
-        <v>151.3374039</v>
+        <f>results!H28</f>
+        <v>0.91048037733076315</v>
       </c>
       <c r="D14">
-        <v>147.81369000000001</v>
+        <f>results!H29</f>
+        <v>1.1191655581289153</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -4769,13 +5776,16 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>105.92256209999999</v>
+        <f>results!H31</f>
+        <v>1.4042359345094091</v>
       </c>
       <c r="C15">
-        <v>248.2098958</v>
+        <f>results!H32</f>
+        <v>2.6454703918131806</v>
       </c>
       <c r="D15">
-        <v>248.3982963</v>
+        <f>results!H33</f>
+        <v>2.6227971109281221</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -4786,13 +5796,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>152.960701</v>
+        <f>results!H35</f>
+        <v>1.9646247544483977</v>
       </c>
       <c r="C16">
-        <v>219.53444160000001</v>
+        <f>results!H36</f>
+        <v>2.5080180089992954</v>
       </c>
       <c r="D16">
-        <v>234.25456199999999</v>
+        <f>results!H37</f>
+        <v>2.6567175277392403</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -4803,13 +5816,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>51.539748699999997</v>
+        <f>results!H39</f>
+        <v>0.91444113536024751</v>
       </c>
       <c r="C17">
-        <v>80.625420899999995</v>
+        <f>results!H40</f>
+        <v>1.1896652524711104</v>
       </c>
       <c r="D17">
-        <v>148.18629569999999</v>
+        <f>results!H41</f>
+        <v>1.7524062179739368</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
@@ -4820,13 +5836,16 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>45.124824099999998</v>
+        <f>results!H43</f>
+        <v>0.87482783034631073</v>
       </c>
       <c r="C18">
-        <v>133.4749631</v>
+        <f>results!H44</f>
+        <v>1.685674910116761</v>
       </c>
       <c r="D18">
-        <v>207.17385379999999</v>
+        <f>results!H45</f>
+        <v>2.2961140965178499</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -4837,13 +5856,16 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>86.830330700000005</v>
+        <f>results!H47</f>
+        <v>1.342800333716601</v>
       </c>
       <c r="C19">
-        <v>164.90622809999999</v>
+        <f>results!H48</f>
+        <v>2.0277442104058219</v>
       </c>
       <c r="D19">
-        <v>244.07273889999999</v>
+        <f>results!H49</f>
+        <v>2.9608404631404954</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -4854,13 +5876,16 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>127.2022891</v>
+        <f>results!H51</f>
+        <v>1.6989176241456923</v>
       </c>
       <c r="C20">
-        <v>217.07579999999999</v>
+        <f>results!H52</f>
+        <v>2.4933072691980787</v>
       </c>
       <c r="D20">
-        <v>243.47557330000001</v>
+        <f>results!H53</f>
+        <v>2.7197363307464149</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -4871,13 +5896,16 @@
         <v>10</v>
       </c>
       <c r="B21">
-        <v>203.9867897</v>
+        <f>results!H55</f>
+        <v>2.3253540748570423</v>
       </c>
       <c r="C21">
-        <v>247.92093080000001</v>
+        <f>results!H56</f>
+        <v>2.6478846944655028</v>
       </c>
       <c r="D21">
-        <v>235.3129453</v>
+        <f>results!H57</f>
+        <v>2.7236794981334151</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -4888,13 +5916,16 @@
         <v>11</v>
       </c>
       <c r="B22">
-        <v>122.237178</v>
+        <f>results!H59</f>
+        <v>1.4716667097826732</v>
       </c>
       <c r="C22">
-        <v>233.1318095</v>
+        <f>results!H60</f>
+        <v>2.7199752044534931</v>
       </c>
       <c r="D22">
-        <v>206.68982539999999</v>
+        <f>results!H61</f>
+        <v>2.362302410485241</v>
       </c>
       <c r="F22" t="s">
         <v>25</v>
@@ -4905,13 +5936,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>41.9432586</v>
+        <f>results!H63</f>
+        <v>0.81409087816313097</v>
       </c>
       <c r="C23">
-        <v>173.8477948</v>
+        <f>results!H64</f>
+        <v>2.1014745495051614</v>
       </c>
       <c r="D23">
-        <v>210.5218366</v>
+        <f>results!H65</f>
+        <v>2.5586365037144478</v>
       </c>
       <c r="F23" t="s">
         <v>19</v>
@@ -4922,13 +5956,16 @@
         <v>34</v>
       </c>
       <c r="B24">
-        <v>188.7527102</v>
+        <f>results!H68</f>
+        <v>2.0634367178920114</v>
       </c>
       <c r="C24">
-        <v>200.4053404</v>
+        <f>results!H69</f>
+        <v>2.1315252448614412</v>
       </c>
       <c r="D24">
-        <v>236.76121449999999</v>
+        <f>results!H70</f>
+        <v>2.43942028006032</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
@@ -4939,16 +5976,36 @@
         <v>35</v>
       </c>
       <c r="B25">
-        <v>58.246919499999997</v>
+        <f>results!H72</f>
+        <v>1.0879060583376314</v>
       </c>
       <c r="C25">
-        <v>111.0645395</v>
+        <f>results!H73</f>
+        <v>1.4682105594929065</v>
       </c>
       <c r="D25">
-        <v>122.9209477</v>
+        <f>results!H74</f>
+        <v>1.6094798116665516</v>
       </c>
       <c r="F25" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26">
+        <f>results!H76</f>
+        <v>1.1117900022085325</v>
+      </c>
+      <c r="C26">
+        <f>results!H77</f>
+        <v>2.2018569416666667</v>
+      </c>
+      <c r="D26">
+        <f>results!H78</f>
+        <v>2.092725887194808</v>
       </c>
     </row>
   </sheetData>
@@ -4957,6 +6014,22 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D94706C8-6849-4739-9DB9-603D1FB3C6CB}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Difficulties!B26:D26</xm:f>
+              <xm:sqref>E26</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{5B2E51A5-F173-4F5B-964B-EE624100270E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>

</xml_diff>

<commit_message>
Changed textures of all tiles. Background and UI still WIP
</commit_message>
<xml_diff>
--- a/Match3_Toolkit/tests/test_results.xlsx
+++ b/Match3_Toolkit/tests/test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\_GAMELAB\BachelorThesis\BA_Match3_Toolkit\Match3_Toolkit\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39013CAD-EDBC-41BB-BF78-D56CF514B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156CFB46-939F-4B4B-8553-F6BA25F462D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
   <si>
     <t xml:space="preserve">					</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>shielded + paint</t>
+  </si>
+  <si>
+    <t>average non-score</t>
+  </si>
+  <si>
+    <t>average score</t>
+  </si>
+  <si>
+    <t>Rounded difficulties of medium configuration</t>
   </si>
 </sst>
 </file>
@@ -663,11 +672,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3378,8 +3390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC0C93A-C015-4CA3-AD87-45AB0AC8DE29}">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3519,7 +3531,7 @@
         <v>0.60026396853331521</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N4:N67" si="3">(C5 - $C$3)/($C$77 - $C$3)</f>
+        <f t="shared" ref="N5:N65" si="3">(C5 - $C$3)/($C$77 - $C$3)</f>
         <v>0.32790338594496743</v>
       </c>
     </row>
@@ -5555,10 +5567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5569,12 +5581,12 @@
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -5584,8 +5596,11 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -5604,8 +5619,22 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <f>ROUND(C3, 3)</f>
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="S3">
+        <f>ROUND(AVERAGE(B3,C3,D3), 3)</f>
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="T3" s="4">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5624,8 +5653,22 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q26" si="0">ROUND(C4, 3)</f>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="R4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S26" si="1">ROUND(AVERAGE(B4,C4,D4), 3)</f>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5644,8 +5687,22 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="T5" s="4">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5664,8 +5721,22 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>1.375</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="1"/>
+        <v>1.256</v>
+      </c>
+      <c r="T6" s="4">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -5684,23 +5755,40 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="1"/>
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="T7" s="4">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="T8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="T10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -5710,8 +5798,9 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -5730,8 +5819,22 @@
       <c r="F12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="R12" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5750,8 +5853,22 @@
       <c r="F13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+      <c r="R13" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -5770,8 +5887,22 @@
       <c r="F14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>0.91</v>
+      </c>
+      <c r="R14" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>0.877</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -5790,8 +5921,22 @@
       <c r="F15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>2.645</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>2.2240000000000002</v>
+      </c>
+      <c r="T15" s="4">
+        <v>13</v>
+      </c>
+      <c r="U15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -5810,8 +5955,22 @@
       <c r="F16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>2.508</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>2.3759999999999999</v>
+      </c>
+      <c r="T16" s="4">
+        <v>15</v>
+      </c>
+      <c r="U16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -5830,8 +5989,22 @@
       <c r="F17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>1.19</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>1.286</v>
+      </c>
+      <c r="T17" s="4">
+        <v>5</v>
+      </c>
+      <c r="U17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -5850,8 +6023,22 @@
       <c r="F18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="1"/>
+        <v>1.619</v>
+      </c>
+      <c r="T18" s="4">
+        <v>7</v>
+      </c>
+      <c r="U18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -5870,8 +6057,22 @@
       <c r="F19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>2.028</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="T19" s="4">
+        <v>10</v>
+      </c>
+      <c r="U19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -5890,8 +6091,22 @@
       <c r="F20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>2.4929999999999999</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="1"/>
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="T20" s="4">
+        <v>14</v>
+      </c>
+      <c r="U20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -5910,8 +6125,22 @@
       <c r="F21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>2.6480000000000001</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="1"/>
+        <v>2.5659999999999998</v>
+      </c>
+      <c r="T21" s="4">
+        <v>16</v>
+      </c>
+      <c r="U21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -5930,8 +6159,22 @@
       <c r="F22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>2.72</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="1"/>
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="T22" s="4">
+        <v>11</v>
+      </c>
+      <c r="U22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -5950,8 +6193,22 @@
       <c r="F23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>2.101</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="1"/>
+        <v>1.825</v>
+      </c>
+      <c r="T23" s="4">
+        <v>9</v>
+      </c>
+      <c r="U23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -5970,8 +6227,22 @@
       <c r="F24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>2.1320000000000001</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="1"/>
+        <v>2.2109999999999999</v>
+      </c>
+      <c r="T24" s="4">
+        <v>12</v>
+      </c>
+      <c r="U24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -5990,8 +6261,22 @@
       <c r="F25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>1.468</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="1"/>
+        <v>1.389</v>
+      </c>
+      <c r="T25" s="4">
+        <v>6</v>
+      </c>
+      <c r="U25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -6006,6 +6291,54 @@
       <c r="D26">
         <f>results!H78</f>
         <v>2.092725887194808</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>2.202</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="1"/>
+        <v>1.802</v>
+      </c>
+      <c r="T26" s="4">
+        <v>8</v>
+      </c>
+      <c r="U26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <f>AVERAGE(B3, B5:B7, B15:B26)</f>
+        <v>1.1955560663439024</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:D30" si="2">AVERAGE(C3, C5:C7, C15:C26)</f>
+        <v>1.8194565619041891</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>2.0482012808820627</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <f>AVERAGE(B4,B12:B14)</f>
+        <v>0.62333689902858025</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:D31" si="3">AVERAGE(C4,C12:C14)</f>
+        <v>0.72505302136752647</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>0.78111202663941648</v>
       </c>
     </row>
   </sheetData>
@@ -6014,7 +6347,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D94706C8-6849-4739-9DB9-603D1FB3C6CB}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{B307B727-FF68-454D-983E-2C2FD666F228}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -6025,28 +6358,24 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Difficulties!B26:D26</xm:f>
-              <xm:sqref>E26</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{5B2E51A5-F173-4F5B-964B-EE624100270E}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Difficulties!B24:D24</xm:f>
-              <xm:sqref>E24</xm:sqref>
+              <xm:f>Difficulties!B3:D3</xm:f>
+              <xm:sqref>E3</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Difficulties!B25:D25</xm:f>
-              <xm:sqref>E25</xm:sqref>
+              <xm:f>Difficulties!B4:D4</xm:f>
+              <xm:sqref>E4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Difficulties!B5:D5</xm:f>
+              <xm:sqref>E5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Difficulties!B6:D6</xm:f>
+              <xm:sqref>E6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Difficulties!B7:D7</xm:f>
+              <xm:sqref>E7</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -6110,7 +6439,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{B307B727-FF68-454D-983E-2C2FD666F228}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{5B2E51A5-F173-4F5B-964B-EE624100270E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -6121,24 +6450,28 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Difficulties!B3:D3</xm:f>
-              <xm:sqref>E3</xm:sqref>
+              <xm:f>Difficulties!B24:D24</xm:f>
+              <xm:sqref>E24</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Difficulties!B4:D4</xm:f>
-              <xm:sqref>E4</xm:sqref>
+              <xm:f>Difficulties!B25:D25</xm:f>
+              <xm:sqref>E25</xm:sqref>
             </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D94706C8-6849-4739-9DB9-603D1FB3C6CB}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Difficulties!B5:D5</xm:f>
-              <xm:sqref>E5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Difficulties!B6:D6</xm:f>
-              <xm:sqref>E6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Difficulties!B7:D7</xm:f>
-              <xm:sqref>E7</xm:sqref>
+              <xm:f>Difficulties!B26:D26</xm:f>
+              <xm:sqref>E26</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>